<commit_message>
Ankona changes 13th Feb 2023- 2nd change
</commit_message>
<xml_diff>
--- a/inst/download/2023-02-01_HealthCanada_Opioid_Table.xlsx
+++ b/inst/download/2023-02-01_HealthCanada_Opioid_Table.xlsx
@@ -1748,7 +1748,7 @@
     <t xml:space="preserve">1971387</t>
   </si>
   <si>
-    <t xml:space="preserve">TRIANAL CÂ½</t>
+    <t xml:space="preserve">TRIANAL C½</t>
   </si>
   <si>
     <t xml:space="preserve">2041626</t>
@@ -2480,7 +2480,7 @@
     <t xml:space="preserve">2242406</t>
   </si>
   <si>
-    <t xml:space="preserve">TRIANAL CÂ¼</t>
+    <t xml:space="preserve">TRIANAL C¼</t>
   </si>
   <si>
     <t xml:space="preserve">2242468</t>

</xml_diff>